<commit_message>
Update section links after MSIS section added
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelley\Documents\Work\COVID-19\inedss-covid19-case-creation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelley\Documents\Work\COVID-19\inedss-covid19-case-entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Demographic</t>
   </si>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -823,9 +823,6 @@
       <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
@@ -833,9 +830,6 @@
       </c>
       <c r="B23" t="s">
         <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
       </c>
       <c r="E23" t="s">
         <v>63</v>

</xml_diff>